<commit_message>
Enter species trait data etc
Also worked on Chao estimator
</commit_message>
<xml_diff>
--- a/PNR_Raw_Data/PNR2022_Aaron_pinned_InvertebrateCommunity.xlsx
+++ b/PNR_Raw_Data/PNR2022_Aaron_pinned_InvertebrateCommunity.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="3167" documentId="11_F25DC773A252ABDACC1048D9019B4AC45ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{245F70FF-5FA6-4685-94DA-A0CC66EF1B63}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2280" yWindow="2270" windowWidth="16470" windowHeight="8530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -1058,10 +1058,10 @@
   <dimension ref="A1:BH193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G180" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N180" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J167" sqref="J167"/>
+      <selection pane="bottomRight" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>